<commit_message>
fix : compute error and improve ui
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasdambreville/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasdambreville/Dev/Perso/wallet_simplify/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4046D0BB-E107-C04A-A47E-66B6B8BD3B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA690D6-6EC4-9344-9A46-90AEAA42B325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="17820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="17820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="49">
   <si>
     <t>MyWallet (Excel) — Template</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>3) la table transaction permet de noter tous les achats et les ventes réalisées</t>
+  </si>
+  <si>
+    <t>priceprice/unit</t>
   </si>
 </sst>
 </file>
@@ -565,7 +568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -728,9 +731,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -755,7 +758,7 @@
         <v>37</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>23</v>

</xml_diff>